<commit_message>
Mejora de la vista oferta
</commit_message>
<xml_diff>
--- a/media/offers/31/offer_C-1-103.xlsx
+++ b/media/offers/31/offer_C-1-103.xlsx
@@ -492,7 +492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C3:I49"/>
+  <dimension ref="C3:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +539,7 @@
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>JIM</t>
+          <t>GIM</t>
         </is>
       </c>
     </row>
@@ -573,14 +573,14 @@
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>2024-10-07</t>
+          <t>2024-10-21</t>
         </is>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1">
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>CONTROLADORES / EXPANSIONES / SUPERVISORES</t>
+          <t>CONTROLADORES / SUPERVISORES / EXPANSIONES</t>
         </is>
       </c>
       <c r="D8" s="5" t="n"/>
@@ -596,163 +596,159 @@
           <t>TAB CONT 01</t>
         </is>
       </c>
+      <c r="D9" s="5" t="n"/>
+      <c r="E9" s="5" t="n"/>
+      <c r="F9" s="5" t="n"/>
+      <c r="G9" s="5" t="n"/>
+      <c r="H9" s="5" t="n"/>
+      <c r="I9" s="6" t="n"/>
     </row>
     <row r="10">
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>MODELO</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>UNIDAD</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>VALOR UNITARIO (USD)</t>
-        </is>
-      </c>
-      <c r="I10" s="2" t="inlineStr">
-        <is>
-          <t>VALOR TOTAL (USD)</t>
-        </is>
+      <c r="C10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>F4-CGM04060</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>Modulo de Control FACILITY EXPLORER F4-CGM04060-0</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="11">
       <c r="C11" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>F4-CGM04060</t>
+          <t>FX-PCX4711-0</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Modulo de Control FACILITY EXPLORER F4-CGM04060-0</t>
+          <t>Modulo de Expansión FACILITY EXPLORER PCX4711</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>UND</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="3" t="n">
+        <v>1930</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>TAB SUPERVISOR</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="n"/>
+      <c r="E12" s="5" t="n"/>
+      <c r="F12" s="5" t="n"/>
+      <c r="G12" s="5" t="n"/>
+      <c r="H12" s="5" t="n"/>
+      <c r="I12" s="6" t="n"/>
+    </row>
+    <row r="13">
+      <c r="C13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>FX80</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>MODULO SUPERVISOR JC FX80</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="n">
         <v>1000</v>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="I13" s="3" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="12">
-      <c r="C12" s="2" t="n">
+    <row r="14">
+      <c r="C14" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>FX-PCX4711-0</t>
-        </is>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>Modulo de Expansión FACILITY EXPLORER PCX4711</t>
-        </is>
-      </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="n">
-        <v>1930</v>
-      </c>
-      <c r="I12" s="3" t="n">
-        <v>1930</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" s="7" t="inlineStr">
-        <is>
-          <t>TAB SUPERVISOR</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>MODELO</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-      <c r="F14" s="2" t="inlineStr">
-        <is>
-          <t>UNIDAD</t>
-        </is>
-      </c>
-      <c r="G14" s="2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="inlineStr">
-        <is>
-          <t>VALOR UNITARIO (USD)</t>
-        </is>
-      </c>
-      <c r="I14" s="2" t="inlineStr">
-        <is>
-          <t>VALOR TOTAL (USD)</t>
-        </is>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>FX-SC8CL005-0</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>Licencia de dispositivo central del controlador de supervisión FX80; 5 dispositivos de campo; 250 puntos</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="15">
       <c r="C15" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>FX80</t>
+          <t>FX-SC8BASE-0</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>MODULO SUPERVISOR JC FX80</t>
+          <t>Controlador de supervisión FX80 y tarjeta micro Secure Digital (SD)</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>UND</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G15" s="3" t="n">
@@ -767,21 +763,21 @@
     </row>
     <row r="16">
       <c r="C16" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>FX-SC8CL005-0</t>
+          <t>FX-SC8D005M1-0</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>Licencia de dispositivo central del controlador de supervisión FX80; 5 dispositivos de campo; 250 puntos</t>
+          <t>Mantenimiento de software inicial de 1 año para el controlador de supervisión FX80 con capacidad de 5–9 dispositivos</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>UND</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G16" s="3" t="n">
@@ -795,352 +791,273 @@
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>SUBTOTAL ( USD)</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="n"/>
+      <c r="G17" s="2" t="n"/>
+      <c r="H17" s="2" t="n"/>
+      <c r="I17" s="2" t="n">
+        <v>6930</v>
+      </c>
+    </row>
+    <row r="19" ht="25" customHeight="1">
+      <c r="C19" s="4" t="inlineStr">
+        <is>
+          <t>INSTRUMENTOS / COFRES</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="n"/>
+      <c r="E19" s="5" t="n"/>
+      <c r="F19" s="5" t="n"/>
+      <c r="G19" s="5" t="n"/>
+      <c r="H19" s="5" t="n"/>
+      <c r="I19" s="6" t="n"/>
+    </row>
+    <row r="20">
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>TAB CONT 01</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="n"/>
+      <c r="E20" s="5" t="n"/>
+      <c r="F20" s="5" t="n"/>
+      <c r="G20" s="5" t="n"/>
+      <c r="H20" s="5" t="n"/>
+      <c r="I20" s="6" t="n"/>
+    </row>
+    <row r="21">
+      <c r="C21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>TR75VA004</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>TRANFORMADOR 75 VA (TR75VA004)</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="I21" s="3" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>AQD-BBBE</t>
+        </is>
+      </c>
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>FX-SC8BASE-0</t>
-        </is>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>Controlador de supervisión FX80 y tarjeta micro Secure Digital (SD)</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I17" s="3" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>FX-SC8D005M1-0</t>
-        </is>
-      </c>
-      <c r="E18" s="3" t="inlineStr">
-        <is>
-          <t>Mantenimiento de software inicial de 1 año para el controlador de supervisión FX80 con capacidad de 5–9 dispositivos</t>
-        </is>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G18" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I18" s="3" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="C19" s="2" t="n"/>
-      <c r="D19" s="2" t="n"/>
-      <c r="E19" s="2" t="inlineStr">
-        <is>
-          <t>SUBTOTAL ( USD)</t>
-        </is>
-      </c>
-      <c r="F19" s="2" t="n"/>
-      <c r="G19" s="2" t="n"/>
-      <c r="H19" s="2" t="n"/>
-      <c r="I19" s="2" t="n">
-        <v>6930</v>
-      </c>
-    </row>
-    <row r="21" ht="25" customHeight="1">
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>INTRUEMENTOS / COFRES</t>
-        </is>
-      </c>
-      <c r="D21" s="5" t="n"/>
-      <c r="E21" s="5" t="n"/>
-      <c r="F21" s="5" t="n"/>
-      <c r="G21" s="5" t="n"/>
-      <c r="H21" s="5" t="n"/>
-      <c r="I21" s="6" t="n"/>
-    </row>
-    <row r="22">
-      <c r="C22" s="7" t="inlineStr">
-        <is>
-          <t>TAB CONT 01</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" s="2" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
-      </c>
-      <c r="D23" s="2" t="inlineStr">
-        <is>
-          <t>MODELO</t>
-        </is>
-      </c>
-      <c r="E23" s="2" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-      <c r="F23" s="2" t="inlineStr">
-        <is>
-          <t>UNIDAD</t>
-        </is>
-      </c>
-      <c r="G23" s="2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
-      <c r="H23" s="2" t="inlineStr">
-        <is>
-          <t>VALOR UNITARIO (USD)</t>
-        </is>
-      </c>
-      <c r="I23" s="2" t="inlineStr">
-        <is>
-          <t>VALOR TOTAL (USD)</t>
-        </is>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>CKIT-VMD1B-C24A</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>RELEVADOR DE 24 VAC; 15 A @ 120 VAC | 15 A @ 28 VDC | 15 A @ 277 VAC</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>16.65</v>
+      </c>
+      <c r="I23" s="3" t="n">
+        <v>33.3</v>
       </c>
     </row>
     <row r="24">
       <c r="C24" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>AQD-BBBE</t>
+          <t>CO5050</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>AQD-BBBE SENSOR DE TEMPERATURA DEL CONDUCTO</t>
+          <t>Cofre Metálico; AUTOSOPORTADO; fabricado en Lamina cold rolled Protección IP-55 Certificación RETIE (Incluye: protecciones; borneras; cableado interno; y marquillado).</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>UND</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G24" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="3" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="I24" s="3" t="n">
-        <v>200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25">
       <c r="C25" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>HT1D</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="inlineStr">
-        <is>
-          <t>TR75VA004</t>
-        </is>
-      </c>
-      <c r="E25" s="3" t="inlineStr">
-        <is>
-          <t>TRANFORMADOR 75 VA (TR75VA004)</t>
-        </is>
-      </c>
-      <c r="F25" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G25" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="H25" s="3" t="n">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="I25" s="3" t="n">
-        <v>47</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26">
-      <c r="C26" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" s="3" t="inlineStr">
-        <is>
-          <t>HT1D</t>
-        </is>
-      </c>
-      <c r="E26" s="3" t="inlineStr">
-        <is>
-          <t>CONDUCTO DE TEMPERATURA DE HUMEDAD</t>
-        </is>
-      </c>
-      <c r="F26" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G26" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H26" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="I26" s="3" t="n">
-        <v>200</v>
-      </c>
+      <c r="C26" s="7" t="inlineStr">
+        <is>
+          <t>TAB SUPERVISOR</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="n"/>
+      <c r="E26" s="5" t="n"/>
+      <c r="F26" s="5" t="n"/>
+      <c r="G26" s="5" t="n"/>
+      <c r="H26" s="5" t="n"/>
+      <c r="I26" s="6" t="n"/>
     </row>
     <row r="27">
       <c r="C27" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>CKIT-VMD1B-C24A</t>
+          <t>TR40VA004</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>RLY KIT-VMD1B-C24A</t>
+          <t>TRANFORMADOR 40 VA (TR40VA004)</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>UND</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G27" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>16.65</v>
+        <v>22</v>
       </c>
       <c r="I27" s="3" t="n">
-        <v>33.3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D28" s="3" t="inlineStr">
-        <is>
-          <t>CO5050</t>
-        </is>
-      </c>
-      <c r="E28" s="3" t="inlineStr">
-        <is>
-          <t>COFRE METALICO DE 50cm x 50cm x 15cm</t>
-        </is>
-      </c>
-      <c r="F28" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G28" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I28" s="3" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D29" s="3" t="inlineStr">
-        <is>
-          <t>P74FA-1C</t>
-        </is>
-      </c>
-      <c r="E29" s="3" t="inlineStr">
-        <is>
-          <t>CONTROL DE PRESIÓN DIFERENCIAL SWITCH</t>
-        </is>
-      </c>
-      <c r="F29" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G29" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H29" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="I29" s="3" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" s="7" t="inlineStr">
-        <is>
-          <t>TAB SUPERVISOR</t>
-        </is>
-      </c>
+      <c r="C28" s="2" t="n"/>
+      <c r="D28" s="2" t="n"/>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>SUBTOTAL ( USD)</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="2" t="n"/>
+      <c r="H28" s="2" t="n"/>
+      <c r="I28" s="2" t="n">
+        <v>1502.3</v>
+      </c>
+    </row>
+    <row r="30" ht="25" customHeight="1">
+      <c r="C30" s="4" t="inlineStr">
+        <is>
+          <t>INGENIERÍA / PROGRAMACIÓN / PUESTA EN OPERACIÓN</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="n"/>
+      <c r="E30" s="5" t="n"/>
+      <c r="F30" s="5" t="n"/>
+      <c r="G30" s="5" t="n"/>
+      <c r="H30" s="5" t="n"/>
+      <c r="I30" s="6" t="n"/>
     </row>
     <row r="31">
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="inlineStr">
-        <is>
-          <t>MODELO</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="inlineStr">
-        <is>
-          <t>UNIDAD</t>
-        </is>
-      </c>
-      <c r="G31" s="2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
-      <c r="H31" s="2" t="inlineStr">
-        <is>
-          <t>VALOR UNITARIO (USD)</t>
-        </is>
-      </c>
-      <c r="I31" s="2" t="inlineStr">
-        <is>
-          <t>VALOR TOTAL (USD)</t>
-        </is>
-      </c>
+      <c r="C31" s="7" t="inlineStr">
+        <is>
+          <t>****</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="n"/>
+      <c r="E31" s="5" t="n"/>
+      <c r="F31" s="5" t="n"/>
+      <c r="G31" s="5" t="n"/>
+      <c r="H31" s="5" t="n"/>
+      <c r="I31" s="6" t="n"/>
     </row>
     <row r="32">
       <c r="C32" s="2" t="n">
@@ -1148,199 +1065,170 @@
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>TR40VA004</t>
+          <t>INGENIERÍA Y PROGRAMACIÓN</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>TRANFORMADOR 40 VA (TR40VA004)</t>
+          <t>Ingeniería de Detalle; Layout; Unifilares y Supervisión. programación de controladores; Planos de taller (Unifilar; Layout tablero; ingeniería de detalle; Manual de operación) Interfaz Grafica</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>863.23</v>
+      </c>
+      <c r="I32" s="3" t="n">
+        <v>863.23</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="inlineStr">
+        <is>
+          <t>PUESTA EN OPERACIÓN DE PROYECTO</t>
+        </is>
+      </c>
+      <c r="E33" s="3" t="inlineStr">
+        <is>
+          <t>Ajuste de parámetro de operación en sitio; Pruebas y Arranque.</t>
+        </is>
+      </c>
+      <c r="F33" s="3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>1294.84</v>
+      </c>
+      <c r="I33" s="3" t="n">
+        <v>1294.84</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D34" s="3" t="inlineStr">
+        <is>
+          <t>P74FA-1C</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>6 A; SPDT; 36 in Cap with 1/4 in Flare Nut; Uni-Directional; PSIG; Liquid/Gas; ±100 psi; Fixed; Switch; 8 - 60 psi; 277 VAC</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="inlineStr">
+        <is>
           <t>UND</t>
         </is>
       </c>
-      <c r="G32" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="3" t="n">
-        <v>22</v>
-      </c>
-      <c r="I32" s="3" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="C33" s="2" t="n"/>
-      <c r="D33" s="2" t="n"/>
-      <c r="E33" s="2" t="inlineStr">
-        <is>
-          <t>SUBTOTAL ( USD )</t>
-        </is>
-      </c>
-      <c r="F33" s="2" t="n"/>
-      <c r="G33" s="2" t="n"/>
-      <c r="H33" s="2" t="n"/>
-      <c r="I33" s="2" t="n">
-        <v>1702.3</v>
-      </c>
-    </row>
-    <row r="35" ht="25" customHeight="1">
-      <c r="C35" s="4" t="inlineStr">
-        <is>
-          <t>INGENIERÍA / PROGRAMACIÓN / PUESTA EN OPERACIÓN</t>
-        </is>
-      </c>
-      <c r="D35" s="5" t="n"/>
-      <c r="E35" s="5" t="n"/>
-      <c r="F35" s="5" t="n"/>
-      <c r="G35" s="5" t="n"/>
-      <c r="H35" s="5" t="n"/>
-      <c r="I35" s="6" t="n"/>
-    </row>
-    <row r="36">
-      <c r="C36" s="2" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
-      </c>
-      <c r="D36" s="2" t="inlineStr">
-        <is>
-          <t>MODELO</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="inlineStr">
-        <is>
-          <t>DESCRIPCIÓN</t>
-        </is>
-      </c>
-      <c r="F36" s="2" t="inlineStr">
-        <is>
-          <t>UNIDAD</t>
-        </is>
-      </c>
-      <c r="G36" s="2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
-      <c r="H36" s="2" t="inlineStr">
-        <is>
-          <t>VALOR UNITARIO (USD)</t>
-        </is>
-      </c>
-      <c r="I36" s="2" t="inlineStr">
-        <is>
-          <t>VALOR TOTAL (USD)</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3" t="inlineStr">
-        <is>
-          <t>INGENIERÍA Y PROGRAMACIÓN</t>
-        </is>
-      </c>
-      <c r="E37" s="3" t="inlineStr">
-        <is>
-          <t>Ingeniería de Detalle; Layout; Unifilares y Supervisión. programación de controladores; Planos de taller (Unifilar; Layout tablero; ingeniería de detalle; Manual de operación) Interfaz Grafica</t>
-        </is>
-      </c>
-      <c r="F37" s="3" t="inlineStr">
+      <c r="G34" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I34" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="2" t="n"/>
+      <c r="D35" s="2" t="n"/>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>SUBTOTAL ( USD)</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="n"/>
+      <c r="G35" s="2" t="n"/>
+      <c r="H35" s="2" t="n"/>
+      <c r="I35" s="2" t="n">
+        <v>2258.07</v>
+      </c>
+    </row>
+    <row r="37" ht="25" customHeight="1">
+      <c r="C37" s="4" t="inlineStr">
+        <is>
+          <t>INSTRUMENTOS ADICIONALES</t>
+        </is>
+      </c>
+      <c r="D37" s="5" t="n"/>
+      <c r="E37" s="5" t="n"/>
+      <c r="F37" s="5" t="n"/>
+      <c r="G37" s="5" t="n"/>
+      <c r="H37" s="5" t="n"/>
+      <c r="I37" s="6" t="n"/>
+    </row>
+    <row r="38">
+      <c r="C38" s="7" t="inlineStr">
+        <is>
+          <t>****</t>
+        </is>
+      </c>
+      <c r="D38" s="5" t="n"/>
+      <c r="E38" s="5" t="n"/>
+      <c r="F38" s="5" t="n"/>
+      <c r="G38" s="5" t="n"/>
+      <c r="H38" s="5" t="n"/>
+      <c r="I38" s="6" t="n"/>
+    </row>
+    <row r="39">
+      <c r="C39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>P74FA-1C</t>
+        </is>
+      </c>
+      <c r="E39" s="3" t="inlineStr">
+        <is>
+          <t>6 A; SPDT; 36 in Cap with 1/4 in Flare Nut; Uni-Directional; PSIG; Liquid/Gas; ±100 psi; Fixed; Switch; 8 - 60 psi; 277 VAC</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="inlineStr">
         <is>
           <t>UND</t>
         </is>
       </c>
-      <c r="G37" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" s="3" t="n">
-        <v>863.23</v>
-      </c>
-      <c r="I37" s="3" t="n">
-        <v>863.23</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="C38" s="2" t="n">
+      <c r="G39" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D38" s="3" t="inlineStr">
-        <is>
-          <t>PUESTA EN OPERACIÓN DE PROYECTO</t>
-        </is>
-      </c>
-      <c r="E38" s="3" t="inlineStr">
-        <is>
-          <t>Ajuste de parámetro de operación en sitio; Pruebas y Arranque.</t>
-        </is>
-      </c>
-      <c r="F38" s="3" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="G38" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" s="3" t="n">
-        <v>1294.84</v>
-      </c>
-      <c r="I38" s="3" t="n">
-        <v>1294.84</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="C39" s="2" t="n"/>
-      <c r="D39" s="2" t="n"/>
-      <c r="E39" s="2" t="inlineStr">
+      <c r="H39" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="I39" s="3" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" s="2" t="n"/>
+      <c r="D40" s="2" t="n"/>
+      <c r="E40" s="2" t="inlineStr">
         <is>
           <t>SUBTOTAL ( USD)</t>
         </is>
       </c>
-      <c r="F39" s="2" t="n"/>
-      <c r="G39" s="2" t="n"/>
-      <c r="H39" s="2" t="n"/>
-      <c r="I39" s="2" t="n">
-        <v>2158.07</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="C41" s="2" t="n"/>
-      <c r="D41" s="2" t="n"/>
-      <c r="E41" s="2" t="inlineStr">
-        <is>
-          <t>SUBTOTAL SUMINISTROS Y DESARROLLO ( USD )</t>
-        </is>
-      </c>
-      <c r="F41" s="2" t="n"/>
-      <c r="G41" s="2" t="n"/>
-      <c r="H41" s="2" t="n"/>
-      <c r="I41" s="2" t="n">
-        <v>10790.37</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="C42" s="2" t="n"/>
-      <c r="D42" s="2" t="n"/>
-      <c r="E42" s="2" t="inlineStr">
-        <is>
-          <t>DESCUENTO</t>
-        </is>
-      </c>
-      <c r="F42" s="2" t="n"/>
-      <c r="G42" s="2" t="n"/>
-      <c r="H42" s="2" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-      <c r="I42" s="2" t="n">
-        <v>0</v>
+      <c r="F40" s="2" t="n"/>
+      <c r="G40" s="2" t="n"/>
+      <c r="H40" s="2" t="n"/>
+      <c r="I40" s="2" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="43">
@@ -1348,14 +1236,14 @@
       <c r="D43" s="2" t="n"/>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>SUBTOTAL MENOS (-) DESCUENTO</t>
+          <t>SUBTOTAL SUMINISTROS Y DESARROLLO ( USD )</t>
         </is>
       </c>
       <c r="F43" s="2" t="n"/>
       <c r="G43" s="2" t="n"/>
       <c r="H43" s="2" t="n"/>
       <c r="I43" s="2" t="n">
-        <v>10790.37</v>
+        <v>10890.37</v>
       </c>
     </row>
     <row r="44">
@@ -1363,18 +1251,18 @@
       <c r="D44" s="2" t="n"/>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>ADMINISTRACIÓN</t>
+          <t>DESCUENTO</t>
         </is>
       </c>
       <c r="F44" s="2" t="n"/>
       <c r="G44" s="2" t="n"/>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>7.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="I44" s="2" t="n">
-        <v>755.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1382,18 +1270,14 @@
       <c r="D45" s="2" t="n"/>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>IMPREVISTROS</t>
+          <t>SUBTOTAL MENOS (-) DESCUENTO</t>
         </is>
       </c>
       <c r="F45" s="2" t="n"/>
       <c r="G45" s="2" t="n"/>
-      <c r="H45" s="2" t="inlineStr">
-        <is>
-          <t>3.0%</t>
-        </is>
-      </c>
+      <c r="H45" s="2" t="n"/>
       <c r="I45" s="2" t="n">
-        <v>323.71</v>
+        <v>10890.37</v>
       </c>
     </row>
     <row r="46">
@@ -1401,18 +1285,18 @@
       <c r="D46" s="2" t="n"/>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>UTILIDADES</t>
+          <t>ADMINISTRACIÓN</t>
         </is>
       </c>
       <c r="F46" s="2" t="n"/>
       <c r="G46" s="2" t="n"/>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>8.0%</t>
+          <t>7.0%</t>
         </is>
       </c>
       <c r="I46" s="2" t="n">
-        <v>863.23</v>
+        <v>762.3259</v>
       </c>
     </row>
     <row r="47">
@@ -1420,14 +1304,18 @@
       <c r="D47" s="2" t="n"/>
       <c r="E47" s="2" t="inlineStr">
         <is>
-          <t>SUBTOTAL COSTO DIRECTO + INDIRECTO</t>
+          <t>IMPREVISTROS</t>
         </is>
       </c>
       <c r="F47" s="2" t="n"/>
       <c r="G47" s="2" t="n"/>
-      <c r="H47" s="2" t="n"/>
+      <c r="H47" s="2" t="inlineStr">
+        <is>
+          <t>3.0%</t>
+        </is>
+      </c>
       <c r="I47" s="2" t="n">
-        <v>12732.64</v>
+        <v>326.7110999999999</v>
       </c>
     </row>
     <row r="48">
@@ -1435,18 +1323,18 @@
       <c r="D48" s="2" t="n"/>
       <c r="E48" s="2" t="inlineStr">
         <is>
-          <t>IVA/UTILIDAD</t>
+          <t>UTILIDADES</t>
         </is>
       </c>
       <c r="F48" s="2" t="n"/>
       <c r="G48" s="2" t="n"/>
       <c r="H48" s="2" t="inlineStr">
         <is>
-          <t>19.0%</t>
+          <t>8.0%</t>
         </is>
       </c>
       <c r="I48" s="2" t="n">
-        <v>2419.201599999999</v>
+        <v>871.2295999999999</v>
       </c>
     </row>
     <row r="49">
@@ -1454,25 +1342,62 @@
       <c r="D49" s="2" t="n"/>
       <c r="E49" s="2" t="inlineStr">
         <is>
-          <t>VALOR TOTAL (USD) DÓLAR ESTADOUNIDENSE</t>
+          <t>SUBTOTAL COSTO DIRECTO + INDIRECTO</t>
         </is>
       </c>
       <c r="F49" s="2" t="n"/>
       <c r="G49" s="2" t="n"/>
       <c r="H49" s="2" t="n"/>
       <c r="I49" s="2" t="n">
-        <v>15151.84</v>
+        <v>12850.6366</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" s="2" t="n"/>
+      <c r="D50" s="2" t="n"/>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>IVA/UTILIDAD</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="n"/>
+      <c r="G50" s="2" t="n"/>
+      <c r="H50" s="2" t="inlineStr">
+        <is>
+          <t>19.0%</t>
+        </is>
+      </c>
+      <c r="I50" s="2" t="n">
+        <v>2441.620954</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="C51" s="2" t="n"/>
+      <c r="D51" s="2" t="n"/>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>VALOR TOTAL (USD) DÓLAR ESTADOUNIDENSE</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="n"/>
+      <c r="G51" s="2" t="n"/>
+      <c r="H51" s="2" t="n"/>
+      <c r="I51" s="2" t="n">
+        <v>15292.257554</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C22:I22"/>
+  <mergeCells count="10">
+    <mergeCell ref="C31:I31"/>
     <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C26:I26"/>
     <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C12:I12"/>
     <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C37:I37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>